<commit_message>
Signed-off-by: Prerk Parikh <pparikh@sigmasolve.net>
</commit_message>
<xml_diff>
--- a/DB Sheet.xlsx
+++ b/DB Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="170">
   <si>
     <t>CompanyId</t>
   </si>
@@ -535,9 +535,6 @@
   </si>
   <si>
     <t>rdppassword</t>
-  </si>
-  <si>
-    <t>dfdf</t>
   </si>
 </sst>
 </file>
@@ -2178,9 +2175,6 @@
       <c r="D5" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">

</xml_diff>